<commit_message>
Python 3 - MM Module Works (Probably)
</commit_message>
<xml_diff>
--- a/_output/MM/(Q1) - Chi-Test - b1 [1]  b5 [1] .xlsx
+++ b/_output/MM/(Q1) - Chi-Test - b1 [1]  b5 [1] .xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="346">
   <si>
     <t>Probability(0.05/0.01/0.001)</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>100.0%</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
   </si>
   <si>
     <t>I engage in the following risky offline activities</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
   <si>
     <t>66.83%</t>
@@ -1476,9 +1470,6 @@
       <c r="C5">
         <v>323.5092144909257</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
       <c r="E5">
         <v>1</v>
       </c>
@@ -1496,37 +1487,34 @@
         <v>402</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
         <v>24</v>
       </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>25</v>
       </c>
-      <c r="N5" t="s">
-        <v>26</v>
-      </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
       <c r="C6">
         <v>322.0859542467583</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -1544,37 +1532,34 @@
         <v>402</v>
       </c>
       <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" t="s">
         <v>29</v>
       </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
       </c>
       <c r="C7">
         <v>12.32082084103385</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -1592,37 +1577,34 @@
         <v>402</v>
       </c>
       <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
         <v>34</v>
       </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>35</v>
       </c>
-      <c r="N7" t="s">
-        <v>36</v>
-      </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
       </c>
       <c r="C8">
         <v>9.955901071439829</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -1640,37 +1622,34 @@
         <v>402</v>
       </c>
       <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
         <v>40</v>
       </c>
-      <c r="K8" t="s">
+      <c r="N8" t="s">
         <v>41</v>
       </c>
-      <c r="L8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" t="s">
-        <v>43</v>
-      </c>
       <c r="O8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>6.170599129181451</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
       <c r="E9">
         <v>1</v>
       </c>
@@ -1688,37 +1667,34 @@
         <v>111</v>
       </c>
       <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" t="s">
         <v>46</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>47</v>
       </c>
-      <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" t="s">
-        <v>49</v>
-      </c>
       <c r="O9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>5.257656711629951</v>
       </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
       <c r="E10">
         <v>1</v>
       </c>
@@ -1736,37 +1712,34 @@
         <v>393</v>
       </c>
       <c r="J10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" t="s">
         <v>52</v>
       </c>
-      <c r="K10" t="s">
+      <c r="N10" t="s">
         <v>53</v>
       </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" t="s">
-        <v>55</v>
-      </c>
       <c r="O10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>5.190748850835965</v>
       </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
       <c r="E11">
         <v>2</v>
       </c>
@@ -1784,37 +1757,34 @@
         <v>402</v>
       </c>
       <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" t="s">
         <v>58</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>59</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>60</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>61</v>
-      </c>
-      <c r="N11" t="s">
-        <v>62</v>
-      </c>
-      <c r="O11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>5.190748850835965</v>
       </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
       <c r="E12">
         <v>2</v>
       </c>
@@ -1832,37 +1802,34 @@
         <v>402</v>
       </c>
       <c r="J12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" t="s">
         <v>58</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>59</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>60</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>61</v>
-      </c>
-      <c r="N12" t="s">
-        <v>62</v>
-      </c>
-      <c r="O12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>4.04144665522562</v>
       </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
       <c r="E13">
         <v>1</v>
       </c>
@@ -1880,22 +1847,22 @@
         <v>399</v>
       </c>
       <c r="J13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
         <v>68</v>
       </c>
-      <c r="K13" t="s">
+      <c r="N13" t="s">
         <v>69</v>
       </c>
-      <c r="L13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" t="s">
-        <v>71</v>
-      </c>
       <c r="O13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1903,14 +1870,11 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>3.484208777016405</v>
       </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
       <c r="E14">
         <v>1</v>
       </c>
@@ -1928,37 +1892,34 @@
         <v>121</v>
       </c>
       <c r="J14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s">
         <v>73</v>
       </c>
-      <c r="K14" t="s">
+      <c r="N14" t="s">
         <v>74</v>
       </c>
-      <c r="L14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" t="s">
-        <v>75</v>
-      </c>
-      <c r="N14" t="s">
-        <v>76</v>
-      </c>
       <c r="O14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15">
         <v>3.268905662871052</v>
       </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
       <c r="E15">
         <v>1</v>
       </c>
@@ -1976,37 +1937,34 @@
         <v>399</v>
       </c>
       <c r="J15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" t="s">
         <v>79</v>
       </c>
-      <c r="K15" t="s">
+      <c r="N15" t="s">
         <v>80</v>
       </c>
-      <c r="L15" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" t="s">
-        <v>81</v>
-      </c>
-      <c r="N15" t="s">
-        <v>82</v>
-      </c>
       <c r="O15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>3.061102026177001</v>
       </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
       <c r="E16">
         <v>1</v>
       </c>
@@ -2024,37 +1982,34 @@
         <v>392</v>
       </c>
       <c r="J16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" t="s">
         <v>85</v>
       </c>
-      <c r="K16" t="s">
+      <c r="N16" t="s">
         <v>86</v>
       </c>
-      <c r="L16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" t="s">
-        <v>87</v>
-      </c>
-      <c r="N16" t="s">
-        <v>88</v>
-      </c>
       <c r="O16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17">
         <v>2.887055048576475</v>
       </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
       <c r="E17">
         <v>1</v>
       </c>
@@ -2072,37 +2027,34 @@
         <v>402</v>
       </c>
       <c r="J17" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" t="s">
+        <v>90</v>
+      </c>
+      <c r="L17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" t="s">
         <v>91</v>
       </c>
-      <c r="K17" t="s">
+      <c r="N17" t="s">
         <v>92</v>
       </c>
-      <c r="L17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" t="s">
-        <v>93</v>
-      </c>
-      <c r="N17" t="s">
-        <v>94</v>
-      </c>
       <c r="O17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C18">
         <v>2.699372118936192</v>
       </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
       <c r="E18">
         <v>1</v>
       </c>
@@ -2120,37 +2072,34 @@
         <v>393</v>
       </c>
       <c r="J18" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" t="s">
         <v>97</v>
       </c>
-      <c r="K18" t="s">
+      <c r="N18" t="s">
         <v>98</v>
       </c>
-      <c r="L18" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" t="s">
-        <v>99</v>
-      </c>
-      <c r="N18" t="s">
-        <v>100</v>
-      </c>
       <c r="O18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19">
         <v>2.506739866332407</v>
       </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
       <c r="E19">
         <v>1</v>
       </c>
@@ -2168,37 +2117,34 @@
         <v>391</v>
       </c>
       <c r="J19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" t="s">
+        <v>102</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" t="s">
         <v>103</v>
       </c>
-      <c r="K19" t="s">
+      <c r="N19" t="s">
         <v>104</v>
       </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" t="s">
-        <v>105</v>
-      </c>
-      <c r="N19" t="s">
-        <v>106</v>
-      </c>
       <c r="O19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C20">
         <v>2.169816657737256</v>
       </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
       <c r="E20">
         <v>1</v>
       </c>
@@ -2216,22 +2162,22 @@
         <v>387</v>
       </c>
       <c r="J20" t="s">
+        <v>107</v>
+      </c>
+      <c r="K20" t="s">
+        <v>108</v>
+      </c>
+      <c r="L20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" t="s">
         <v>109</v>
       </c>
-      <c r="K20" t="s">
+      <c r="N20" t="s">
         <v>110</v>
       </c>
-      <c r="L20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" t="s">
-        <v>111</v>
-      </c>
-      <c r="N20" t="s">
-        <v>112</v>
-      </c>
       <c r="O20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2239,14 +2185,11 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21">
         <v>2.088871667180926</v>
       </c>
-      <c r="D21" t="s">
-        <v>39</v>
-      </c>
       <c r="E21">
         <v>1</v>
       </c>
@@ -2264,37 +2207,34 @@
         <v>123</v>
       </c>
       <c r="J21" t="s">
+        <v>112</v>
+      </c>
+      <c r="K21" t="s">
+        <v>113</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" t="s">
         <v>114</v>
       </c>
-      <c r="K21" t="s">
+      <c r="N21" t="s">
         <v>115</v>
       </c>
-      <c r="L21" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" t="s">
-        <v>116</v>
-      </c>
-      <c r="N21" t="s">
-        <v>117</v>
-      </c>
       <c r="O21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C22">
         <v>2.010055891221569</v>
       </c>
-      <c r="D22" t="s">
-        <v>22</v>
-      </c>
       <c r="E22">
         <v>1</v>
       </c>
@@ -2312,37 +2252,34 @@
         <v>109</v>
       </c>
       <c r="J22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" t="s">
+        <v>119</v>
+      </c>
+      <c r="L22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" t="s">
         <v>120</v>
       </c>
-      <c r="K22" t="s">
+      <c r="N22" t="s">
         <v>121</v>
       </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" t="s">
-        <v>122</v>
-      </c>
-      <c r="N22" t="s">
-        <v>123</v>
-      </c>
       <c r="O22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C23">
         <v>1.674614334294349</v>
       </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
       <c r="E23">
         <v>1</v>
       </c>
@@ -2360,37 +2297,34 @@
         <v>373</v>
       </c>
       <c r="J23" t="s">
+        <v>124</v>
+      </c>
+      <c r="K23" t="s">
+        <v>125</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s">
         <v>126</v>
       </c>
-      <c r="K23" t="s">
+      <c r="N23" t="s">
         <v>127</v>
       </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" t="s">
-        <v>128</v>
-      </c>
-      <c r="N23" t="s">
-        <v>129</v>
-      </c>
       <c r="O23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C24">
         <v>1.571705350874635</v>
       </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
       <c r="E24">
         <v>1</v>
       </c>
@@ -2408,37 +2342,34 @@
         <v>396</v>
       </c>
       <c r="J24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C25">
         <v>1.505841778612141</v>
       </c>
-      <c r="D25" t="s">
-        <v>39</v>
-      </c>
       <c r="E25">
         <v>1</v>
       </c>
@@ -2456,37 +2387,34 @@
         <v>397</v>
       </c>
       <c r="J25" t="s">
+        <v>134</v>
+      </c>
+      <c r="K25" t="s">
+        <v>135</v>
+      </c>
+      <c r="L25" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" t="s">
         <v>136</v>
       </c>
-      <c r="K25" t="s">
+      <c r="N25" t="s">
         <v>137</v>
       </c>
-      <c r="L25" t="s">
-        <v>24</v>
-      </c>
-      <c r="M25" t="s">
-        <v>138</v>
-      </c>
-      <c r="N25" t="s">
-        <v>139</v>
-      </c>
       <c r="O25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26">
         <v>1.412760814693464</v>
       </c>
-      <c r="D26" t="s">
-        <v>22</v>
-      </c>
       <c r="E26">
         <v>1</v>
       </c>
@@ -2504,37 +2432,34 @@
         <v>402</v>
       </c>
       <c r="J26" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" t="s">
         <v>142</v>
       </c>
-      <c r="K26" t="s">
+      <c r="N26" t="s">
         <v>143</v>
       </c>
-      <c r="L26" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26" t="s">
-        <v>144</v>
-      </c>
-      <c r="N26" t="s">
-        <v>145</v>
-      </c>
       <c r="O26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C27">
         <v>1.40249144842308</v>
       </c>
-      <c r="D27" t="s">
-        <v>22</v>
-      </c>
       <c r="E27">
         <v>1</v>
       </c>
@@ -2552,37 +2477,34 @@
         <v>402</v>
       </c>
       <c r="J27" t="s">
+        <v>146</v>
+      </c>
+      <c r="K27" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" t="s">
         <v>148</v>
       </c>
-      <c r="K27" t="s">
+      <c r="N27" t="s">
         <v>149</v>
       </c>
-      <c r="L27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" t="s">
-        <v>150</v>
-      </c>
-      <c r="N27" t="s">
-        <v>151</v>
-      </c>
       <c r="O27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C28">
         <v>1.201456101213009</v>
       </c>
-      <c r="D28" t="s">
-        <v>22</v>
-      </c>
       <c r="E28">
         <v>1</v>
       </c>
@@ -2600,37 +2522,34 @@
         <v>397</v>
       </c>
       <c r="J28" t="s">
+        <v>152</v>
+      </c>
+      <c r="K28" t="s">
+        <v>153</v>
+      </c>
+      <c r="L28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" t="s">
         <v>154</v>
       </c>
-      <c r="K28" t="s">
+      <c r="N28" t="s">
         <v>155</v>
       </c>
-      <c r="L28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" t="s">
-        <v>156</v>
-      </c>
-      <c r="N28" t="s">
-        <v>157</v>
-      </c>
       <c r="O28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29">
         <v>1.171807235793538</v>
       </c>
-      <c r="D29" t="s">
-        <v>39</v>
-      </c>
       <c r="E29">
         <v>1</v>
       </c>
@@ -2648,37 +2567,34 @@
         <v>398</v>
       </c>
       <c r="J29" t="s">
+        <v>158</v>
+      </c>
+      <c r="K29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L29" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" t="s">
         <v>160</v>
       </c>
-      <c r="K29" t="s">
+      <c r="N29" t="s">
         <v>161</v>
       </c>
-      <c r="L29" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" t="s">
-        <v>162</v>
-      </c>
-      <c r="N29" t="s">
-        <v>163</v>
-      </c>
       <c r="O29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C30">
         <v>1.053008432777665</v>
       </c>
-      <c r="D30" t="s">
-        <v>22</v>
-      </c>
       <c r="E30">
         <v>1</v>
       </c>
@@ -2696,37 +2612,34 @@
         <v>401</v>
       </c>
       <c r="J30" t="s">
+        <v>164</v>
+      </c>
+      <c r="K30" t="s">
+        <v>165</v>
+      </c>
+      <c r="L30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30" t="s">
         <v>166</v>
       </c>
-      <c r="K30" t="s">
+      <c r="N30" t="s">
         <v>167</v>
       </c>
-      <c r="L30" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" t="s">
-        <v>168</v>
-      </c>
-      <c r="N30" t="s">
-        <v>169</v>
-      </c>
       <c r="O30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C31">
         <v>1.029937178549565</v>
       </c>
-      <c r="D31" t="s">
-        <v>39</v>
-      </c>
       <c r="E31">
         <v>1</v>
       </c>
@@ -2744,37 +2657,34 @@
         <v>401</v>
       </c>
       <c r="J31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K31" t="s">
+        <v>171</v>
+      </c>
+      <c r="L31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" t="s">
         <v>172</v>
       </c>
-      <c r="K31" t="s">
+      <c r="N31" t="s">
         <v>173</v>
       </c>
-      <c r="L31" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" t="s">
-        <v>174</v>
-      </c>
-      <c r="N31" t="s">
-        <v>175</v>
-      </c>
       <c r="O31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C32">
         <v>0.9646498126970781</v>
       </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
       <c r="E32">
         <v>1</v>
       </c>
@@ -2792,37 +2702,34 @@
         <v>402</v>
       </c>
       <c r="J32" t="s">
+        <v>176</v>
+      </c>
+      <c r="K32" t="s">
+        <v>177</v>
+      </c>
+      <c r="L32" t="s">
+        <v>23</v>
+      </c>
+      <c r="M32" t="s">
         <v>178</v>
       </c>
-      <c r="K32" t="s">
+      <c r="N32" t="s">
         <v>179</v>
       </c>
-      <c r="L32" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" t="s">
-        <v>180</v>
-      </c>
-      <c r="N32" t="s">
-        <v>181</v>
-      </c>
       <c r="O32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C33">
         <v>0.9573186746203201</v>
       </c>
-      <c r="D33" t="s">
-        <v>22</v>
-      </c>
       <c r="E33">
         <v>1</v>
       </c>
@@ -2840,37 +2747,34 @@
         <v>390</v>
       </c>
       <c r="J33" t="s">
+        <v>182</v>
+      </c>
+      <c r="K33" t="s">
+        <v>183</v>
+      </c>
+      <c r="L33" t="s">
+        <v>23</v>
+      </c>
+      <c r="M33" t="s">
         <v>184</v>
       </c>
-      <c r="K33" t="s">
+      <c r="N33" t="s">
         <v>185</v>
       </c>
-      <c r="L33" t="s">
-        <v>24</v>
-      </c>
-      <c r="M33" t="s">
-        <v>186</v>
-      </c>
-      <c r="N33" t="s">
-        <v>187</v>
-      </c>
       <c r="O33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C34">
         <v>0.7502601301429429</v>
       </c>
-      <c r="D34" t="s">
-        <v>39</v>
-      </c>
       <c r="E34">
         <v>1</v>
       </c>
@@ -2888,37 +2792,34 @@
         <v>385</v>
       </c>
       <c r="J34" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" t="s">
+        <v>189</v>
+      </c>
+      <c r="L34" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" t="s">
         <v>190</v>
       </c>
-      <c r="K34" t="s">
+      <c r="N34" t="s">
         <v>191</v>
       </c>
-      <c r="L34" t="s">
-        <v>24</v>
-      </c>
-      <c r="M34" t="s">
-        <v>192</v>
-      </c>
-      <c r="N34" t="s">
-        <v>193</v>
-      </c>
       <c r="O34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C35">
         <v>0.6184877964326578</v>
       </c>
-      <c r="D35" t="s">
-        <v>39</v>
-      </c>
       <c r="E35">
         <v>1</v>
       </c>
@@ -2936,37 +2837,34 @@
         <v>396</v>
       </c>
       <c r="J35" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" t="s">
+        <v>195</v>
+      </c>
+      <c r="L35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" t="s">
         <v>196</v>
       </c>
-      <c r="K35" t="s">
+      <c r="N35" t="s">
         <v>197</v>
       </c>
-      <c r="L35" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" t="s">
-        <v>198</v>
-      </c>
-      <c r="N35" t="s">
-        <v>199</v>
-      </c>
       <c r="O35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C36">
         <v>0.6181514123143013</v>
       </c>
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
       <c r="E36">
         <v>1</v>
       </c>
@@ -2984,37 +2882,34 @@
         <v>399</v>
       </c>
       <c r="J36" t="s">
+        <v>200</v>
+      </c>
+      <c r="K36" t="s">
+        <v>201</v>
+      </c>
+      <c r="L36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" t="s">
         <v>202</v>
       </c>
-      <c r="K36" t="s">
+      <c r="N36" t="s">
         <v>203</v>
       </c>
-      <c r="L36" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" t="s">
-        <v>204</v>
-      </c>
-      <c r="N36" t="s">
-        <v>205</v>
-      </c>
       <c r="O36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C37">
         <v>0.5417293835603155</v>
       </c>
-      <c r="D37" t="s">
-        <v>22</v>
-      </c>
       <c r="E37">
         <v>1</v>
       </c>
@@ -3032,37 +2927,34 @@
         <v>401</v>
       </c>
       <c r="J37" t="s">
+        <v>206</v>
+      </c>
+      <c r="K37" t="s">
+        <v>207</v>
+      </c>
+      <c r="L37" t="s">
+        <v>23</v>
+      </c>
+      <c r="M37" t="s">
         <v>208</v>
       </c>
-      <c r="K37" t="s">
+      <c r="N37" t="s">
         <v>209</v>
       </c>
-      <c r="L37" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" t="s">
-        <v>210</v>
-      </c>
-      <c r="N37" t="s">
-        <v>211</v>
-      </c>
       <c r="O37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C38">
         <v>0.4482407836171069</v>
       </c>
-      <c r="D38" t="s">
-        <v>22</v>
-      </c>
       <c r="E38">
         <v>1</v>
       </c>
@@ -3080,37 +2972,34 @@
         <v>398</v>
       </c>
       <c r="J38" t="s">
+        <v>212</v>
+      </c>
+      <c r="K38" t="s">
+        <v>213</v>
+      </c>
+      <c r="L38" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" t="s">
         <v>214</v>
       </c>
-      <c r="K38" t="s">
+      <c r="N38" t="s">
         <v>215</v>
       </c>
-      <c r="L38" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" t="s">
-        <v>216</v>
-      </c>
-      <c r="N38" t="s">
-        <v>217</v>
-      </c>
       <c r="O38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B39" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C39">
         <v>0.333161482190207</v>
       </c>
-      <c r="D39" t="s">
-        <v>22</v>
-      </c>
       <c r="E39">
         <v>1</v>
       </c>
@@ -3128,37 +3017,34 @@
         <v>402</v>
       </c>
       <c r="J39" t="s">
+        <v>218</v>
+      </c>
+      <c r="K39" t="s">
+        <v>219</v>
+      </c>
+      <c r="L39" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" t="s">
         <v>220</v>
       </c>
-      <c r="K39" t="s">
+      <c r="N39" t="s">
         <v>221</v>
       </c>
-      <c r="L39" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" t="s">
-        <v>222</v>
-      </c>
-      <c r="N39" t="s">
-        <v>223</v>
-      </c>
       <c r="O39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B40" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C40">
         <v>0.2932539178137442</v>
       </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
       <c r="E40">
         <v>1</v>
       </c>
@@ -3176,37 +3062,34 @@
         <v>399</v>
       </c>
       <c r="J40" t="s">
+        <v>224</v>
+      </c>
+      <c r="K40" t="s">
+        <v>225</v>
+      </c>
+      <c r="L40" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" t="s">
         <v>226</v>
       </c>
-      <c r="K40" t="s">
+      <c r="N40" t="s">
         <v>227</v>
       </c>
-      <c r="L40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M40" t="s">
-        <v>228</v>
-      </c>
-      <c r="N40" t="s">
-        <v>229</v>
-      </c>
       <c r="O40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C41">
         <v>0.271794967039105</v>
       </c>
-      <c r="D41" t="s">
-        <v>22</v>
-      </c>
       <c r="E41">
         <v>1</v>
       </c>
@@ -3224,37 +3107,34 @@
         <v>402</v>
       </c>
       <c r="J41" t="s">
+        <v>230</v>
+      </c>
+      <c r="K41" t="s">
+        <v>231</v>
+      </c>
+      <c r="L41" t="s">
+        <v>23</v>
+      </c>
+      <c r="M41" t="s">
         <v>232</v>
       </c>
-      <c r="K41" t="s">
+      <c r="N41" t="s">
         <v>233</v>
       </c>
-      <c r="L41" t="s">
-        <v>24</v>
-      </c>
-      <c r="M41" t="s">
-        <v>234</v>
-      </c>
-      <c r="N41" t="s">
-        <v>235</v>
-      </c>
       <c r="O41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B42" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C42">
         <v>0.2674573172835039</v>
       </c>
-      <c r="D42" t="s">
-        <v>39</v>
-      </c>
       <c r="E42">
         <v>1</v>
       </c>
@@ -3272,37 +3152,34 @@
         <v>397</v>
       </c>
       <c r="J42" t="s">
+        <v>236</v>
+      </c>
+      <c r="K42" t="s">
+        <v>237</v>
+      </c>
+      <c r="L42" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" t="s">
         <v>238</v>
       </c>
-      <c r="K42" t="s">
+      <c r="N42" t="s">
         <v>239</v>
       </c>
-      <c r="L42" t="s">
-        <v>24</v>
-      </c>
-      <c r="M42" t="s">
-        <v>240</v>
-      </c>
-      <c r="N42" t="s">
-        <v>241</v>
-      </c>
       <c r="O42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B43" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C43">
         <v>0.2653968029271215</v>
       </c>
-      <c r="D43" t="s">
-        <v>22</v>
-      </c>
       <c r="E43">
         <v>1</v>
       </c>
@@ -3320,37 +3197,34 @@
         <v>402</v>
       </c>
       <c r="J43" t="s">
+        <v>242</v>
+      </c>
+      <c r="K43" t="s">
+        <v>243</v>
+      </c>
+      <c r="L43" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43" t="s">
         <v>244</v>
       </c>
-      <c r="K43" t="s">
+      <c r="N43" t="s">
         <v>245</v>
       </c>
-      <c r="L43" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" t="s">
-        <v>246</v>
-      </c>
-      <c r="N43" t="s">
-        <v>247</v>
-      </c>
       <c r="O43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C44">
         <v>0.257117746363643</v>
       </c>
-      <c r="D44" t="s">
-        <v>22</v>
-      </c>
       <c r="E44">
         <v>1</v>
       </c>
@@ -3368,37 +3242,34 @@
         <v>392</v>
       </c>
       <c r="J44" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M44" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N44" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B45" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C45">
         <v>0.2131689575760013</v>
       </c>
-      <c r="D45" t="s">
-        <v>22</v>
-      </c>
       <c r="E45">
         <v>1</v>
       </c>
@@ -3416,37 +3287,34 @@
         <v>119</v>
       </c>
       <c r="J45" t="s">
+        <v>252</v>
+      </c>
+      <c r="K45" t="s">
+        <v>253</v>
+      </c>
+      <c r="L45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45" t="s">
         <v>254</v>
       </c>
-      <c r="K45" t="s">
+      <c r="N45" t="s">
         <v>255</v>
       </c>
-      <c r="L45" t="s">
-        <v>24</v>
-      </c>
-      <c r="M45" t="s">
-        <v>256</v>
-      </c>
-      <c r="N45" t="s">
-        <v>257</v>
-      </c>
       <c r="O45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B46" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C46">
         <v>0.1720408932919261</v>
       </c>
-      <c r="D46" t="s">
-        <v>39</v>
-      </c>
       <c r="E46">
         <v>1</v>
       </c>
@@ -3464,37 +3332,34 @@
         <v>399</v>
       </c>
       <c r="J46" t="s">
+        <v>258</v>
+      </c>
+      <c r="K46" t="s">
+        <v>259</v>
+      </c>
+      <c r="L46" t="s">
+        <v>23</v>
+      </c>
+      <c r="M46" t="s">
         <v>260</v>
       </c>
-      <c r="K46" t="s">
+      <c r="N46" t="s">
         <v>261</v>
       </c>
-      <c r="L46" t="s">
-        <v>24</v>
-      </c>
-      <c r="M46" t="s">
-        <v>262</v>
-      </c>
-      <c r="N46" t="s">
-        <v>263</v>
-      </c>
       <c r="O46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C47">
         <v>0.1222857154218466</v>
       </c>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
       <c r="E47">
         <v>1</v>
       </c>
@@ -3512,37 +3377,34 @@
         <v>401</v>
       </c>
       <c r="J47" t="s">
+        <v>264</v>
+      </c>
+      <c r="K47" t="s">
+        <v>265</v>
+      </c>
+      <c r="L47" t="s">
+        <v>23</v>
+      </c>
+      <c r="M47" t="s">
         <v>266</v>
       </c>
-      <c r="K47" t="s">
+      <c r="N47" t="s">
         <v>267</v>
       </c>
-      <c r="L47" t="s">
-        <v>24</v>
-      </c>
-      <c r="M47" t="s">
-        <v>268</v>
-      </c>
-      <c r="N47" t="s">
-        <v>269</v>
-      </c>
       <c r="O47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:15">
       <c r="A48" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B48" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C48">
         <v>0.1163360558838181</v>
       </c>
-      <c r="D48" t="s">
-        <v>39</v>
-      </c>
       <c r="E48">
         <v>1</v>
       </c>
@@ -3560,37 +3422,34 @@
         <v>396</v>
       </c>
       <c r="J48" t="s">
+        <v>270</v>
+      </c>
+      <c r="K48" t="s">
+        <v>271</v>
+      </c>
+      <c r="L48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" t="s">
         <v>272</v>
       </c>
-      <c r="K48" t="s">
+      <c r="N48" t="s">
         <v>273</v>
       </c>
-      <c r="L48" t="s">
-        <v>24</v>
-      </c>
-      <c r="M48" t="s">
-        <v>274</v>
-      </c>
-      <c r="N48" t="s">
-        <v>275</v>
-      </c>
       <c r="O48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B49" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C49">
         <v>0.09193293815964224</v>
       </c>
-      <c r="D49" t="s">
-        <v>39</v>
-      </c>
       <c r="E49">
         <v>1</v>
       </c>
@@ -3608,37 +3467,34 @@
         <v>400</v>
       </c>
       <c r="J49" t="s">
+        <v>276</v>
+      </c>
+      <c r="K49" t="s">
+        <v>277</v>
+      </c>
+      <c r="L49" t="s">
+        <v>23</v>
+      </c>
+      <c r="M49" t="s">
         <v>278</v>
       </c>
-      <c r="K49" t="s">
+      <c r="N49" t="s">
         <v>279</v>
       </c>
-      <c r="L49" t="s">
-        <v>24</v>
-      </c>
-      <c r="M49" t="s">
-        <v>280</v>
-      </c>
-      <c r="N49" t="s">
-        <v>281</v>
-      </c>
       <c r="O49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B50" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C50">
         <v>0.07799178148881254</v>
       </c>
-      <c r="D50" t="s">
-        <v>22</v>
-      </c>
       <c r="E50">
         <v>1</v>
       </c>
@@ -3656,37 +3512,34 @@
         <v>399</v>
       </c>
       <c r="J50" t="s">
+        <v>282</v>
+      </c>
+      <c r="K50" t="s">
+        <v>283</v>
+      </c>
+      <c r="L50" t="s">
+        <v>23</v>
+      </c>
+      <c r="M50" t="s">
         <v>284</v>
       </c>
-      <c r="K50" t="s">
+      <c r="N50" t="s">
         <v>285</v>
       </c>
-      <c r="L50" t="s">
-        <v>24</v>
-      </c>
-      <c r="M50" t="s">
-        <v>286</v>
-      </c>
-      <c r="N50" t="s">
-        <v>287</v>
-      </c>
       <c r="O50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C51">
         <v>0.05017669301381705</v>
       </c>
-      <c r="D51" t="s">
-        <v>22</v>
-      </c>
       <c r="E51">
         <v>1</v>
       </c>
@@ -3704,37 +3557,34 @@
         <v>402</v>
       </c>
       <c r="J51" t="s">
+        <v>288</v>
+      </c>
+      <c r="K51" t="s">
+        <v>289</v>
+      </c>
+      <c r="L51" t="s">
+        <v>23</v>
+      </c>
+      <c r="M51" t="s">
         <v>290</v>
       </c>
-      <c r="K51" t="s">
+      <c r="N51" t="s">
         <v>291</v>
       </c>
-      <c r="L51" t="s">
-        <v>24</v>
-      </c>
-      <c r="M51" t="s">
-        <v>292</v>
-      </c>
-      <c r="N51" t="s">
-        <v>293</v>
-      </c>
       <c r="O51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B52" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C52">
         <v>0.04058353886922682</v>
       </c>
-      <c r="D52" t="s">
-        <v>39</v>
-      </c>
       <c r="E52">
         <v>1</v>
       </c>
@@ -3752,37 +3602,34 @@
         <v>401</v>
       </c>
       <c r="J52" t="s">
+        <v>294</v>
+      </c>
+      <c r="K52" t="s">
+        <v>295</v>
+      </c>
+      <c r="L52" t="s">
+        <v>23</v>
+      </c>
+      <c r="M52" t="s">
         <v>296</v>
       </c>
-      <c r="K52" t="s">
+      <c r="N52" t="s">
         <v>297</v>
       </c>
-      <c r="L52" t="s">
-        <v>24</v>
-      </c>
-      <c r="M52" t="s">
-        <v>298</v>
-      </c>
-      <c r="N52" t="s">
-        <v>299</v>
-      </c>
       <c r="O52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B53" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C53">
         <v>0.0379046309677346</v>
       </c>
-      <c r="D53" t="s">
-        <v>39</v>
-      </c>
       <c r="E53">
         <v>1</v>
       </c>
@@ -3800,37 +3647,34 @@
         <v>379</v>
       </c>
       <c r="J53" t="s">
+        <v>300</v>
+      </c>
+      <c r="K53" t="s">
+        <v>301</v>
+      </c>
+      <c r="L53" t="s">
+        <v>23</v>
+      </c>
+      <c r="M53" t="s">
         <v>302</v>
       </c>
-      <c r="K53" t="s">
+      <c r="N53" t="s">
         <v>303</v>
       </c>
-      <c r="L53" t="s">
-        <v>24</v>
-      </c>
-      <c r="M53" t="s">
-        <v>304</v>
-      </c>
-      <c r="N53" t="s">
-        <v>305</v>
-      </c>
       <c r="O53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B54" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C54">
         <v>0.03726816435927848</v>
       </c>
-      <c r="D54" t="s">
-        <v>39</v>
-      </c>
       <c r="E54">
         <v>1</v>
       </c>
@@ -3848,37 +3692,34 @@
         <v>398</v>
       </c>
       <c r="J54" t="s">
+        <v>306</v>
+      </c>
+      <c r="K54" t="s">
+        <v>307</v>
+      </c>
+      <c r="L54" t="s">
+        <v>23</v>
+      </c>
+      <c r="M54" t="s">
         <v>308</v>
       </c>
-      <c r="K54" t="s">
+      <c r="N54" t="s">
         <v>309</v>
       </c>
-      <c r="L54" t="s">
-        <v>24</v>
-      </c>
-      <c r="M54" t="s">
-        <v>310</v>
-      </c>
-      <c r="N54" t="s">
-        <v>311</v>
-      </c>
       <c r="O54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C55">
         <v>0.03199222895642787</v>
       </c>
-      <c r="D55" t="s">
-        <v>39</v>
-      </c>
       <c r="E55">
         <v>1</v>
       </c>
@@ -3896,37 +3737,34 @@
         <v>399</v>
       </c>
       <c r="J55" t="s">
+        <v>312</v>
+      </c>
+      <c r="K55" t="s">
+        <v>313</v>
+      </c>
+      <c r="L55" t="s">
+        <v>23</v>
+      </c>
+      <c r="M55" t="s">
         <v>314</v>
       </c>
-      <c r="K55" t="s">
+      <c r="N55" t="s">
         <v>315</v>
       </c>
-      <c r="L55" t="s">
-        <v>24</v>
-      </c>
-      <c r="M55" t="s">
-        <v>316</v>
-      </c>
-      <c r="N55" t="s">
-        <v>317</v>
-      </c>
       <c r="O55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B56" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C56">
         <v>0.02180668727913699</v>
       </c>
-      <c r="D56" t="s">
-        <v>22</v>
-      </c>
       <c r="E56">
         <v>1</v>
       </c>
@@ -3944,37 +3782,34 @@
         <v>401</v>
       </c>
       <c r="J56" t="s">
+        <v>318</v>
+      </c>
+      <c r="K56" t="s">
+        <v>319</v>
+      </c>
+      <c r="L56" t="s">
+        <v>23</v>
+      </c>
+      <c r="M56" t="s">
         <v>320</v>
       </c>
-      <c r="K56" t="s">
+      <c r="N56" t="s">
         <v>321</v>
       </c>
-      <c r="L56" t="s">
-        <v>24</v>
-      </c>
-      <c r="M56" t="s">
-        <v>322</v>
-      </c>
-      <c r="N56" t="s">
-        <v>323</v>
-      </c>
       <c r="O56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B57" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C57">
         <v>0.01083114056659436</v>
       </c>
-      <c r="D57" t="s">
-        <v>39</v>
-      </c>
       <c r="E57">
         <v>1</v>
       </c>
@@ -3992,37 +3827,34 @@
         <v>392</v>
       </c>
       <c r="J57" t="s">
+        <v>324</v>
+      </c>
+      <c r="K57" t="s">
+        <v>325</v>
+      </c>
+      <c r="L57" t="s">
+        <v>23</v>
+      </c>
+      <c r="M57" t="s">
         <v>326</v>
       </c>
-      <c r="K57" t="s">
+      <c r="N57" t="s">
         <v>327</v>
       </c>
-      <c r="L57" t="s">
-        <v>24</v>
-      </c>
-      <c r="M57" t="s">
-        <v>328</v>
-      </c>
-      <c r="N57" t="s">
-        <v>329</v>
-      </c>
       <c r="O57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B58" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C58">
         <v>0.006589927186998508</v>
       </c>
-      <c r="D58" t="s">
-        <v>22</v>
-      </c>
       <c r="E58">
         <v>1</v>
       </c>
@@ -4040,37 +3872,34 @@
         <v>402</v>
       </c>
       <c r="J58" t="s">
+        <v>330</v>
+      </c>
+      <c r="K58" t="s">
+        <v>331</v>
+      </c>
+      <c r="L58" t="s">
+        <v>23</v>
+      </c>
+      <c r="M58" t="s">
         <v>332</v>
       </c>
-      <c r="K58" t="s">
+      <c r="N58" t="s">
         <v>333</v>
       </c>
-      <c r="L58" t="s">
-        <v>24</v>
-      </c>
-      <c r="M58" t="s">
-        <v>334</v>
-      </c>
-      <c r="N58" t="s">
-        <v>335</v>
-      </c>
       <c r="O58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B59" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C59">
         <v>0.005513595702805824</v>
       </c>
-      <c r="D59" t="s">
-        <v>39</v>
-      </c>
       <c r="E59">
         <v>1</v>
       </c>
@@ -4088,37 +3917,34 @@
         <v>388</v>
       </c>
       <c r="J59" t="s">
+        <v>336</v>
+      </c>
+      <c r="K59" t="s">
+        <v>337</v>
+      </c>
+      <c r="L59" t="s">
+        <v>23</v>
+      </c>
+      <c r="M59" t="s">
         <v>338</v>
       </c>
-      <c r="K59" t="s">
+      <c r="N59" t="s">
         <v>339</v>
       </c>
-      <c r="L59" t="s">
-        <v>24</v>
-      </c>
-      <c r="M59" t="s">
-        <v>340</v>
-      </c>
-      <c r="N59" t="s">
-        <v>341</v>
-      </c>
       <c r="O59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B60" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C60">
         <v>0.0002430083696029905</v>
       </c>
-      <c r="D60" t="s">
-        <v>22</v>
-      </c>
       <c r="E60">
         <v>1</v>
       </c>
@@ -4136,22 +3962,22 @@
         <v>395</v>
       </c>
       <c r="J60" t="s">
+        <v>342</v>
+      </c>
+      <c r="K60" t="s">
+        <v>343</v>
+      </c>
+      <c r="L60" t="s">
+        <v>23</v>
+      </c>
+      <c r="M60" t="s">
         <v>344</v>
       </c>
-      <c r="K60" t="s">
+      <c r="N60" t="s">
         <v>345</v>
       </c>
-      <c r="L60" t="s">
-        <v>24</v>
-      </c>
-      <c r="M60" t="s">
-        <v>346</v>
-      </c>
-      <c r="N60" t="s">
-        <v>347</v>
-      </c>
       <c r="O60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>